<commit_message>
update caravel FTDI mainboard V4 (Rev 4B)
</commit_message>
<xml_diff>
--- a/hardware/caravel_pcb_v4_FTDI/caravel_pcb_v4_FTDI.xlsx
+++ b/hardware/caravel_pcb_v4_FTDI/caravel_pcb_v4_FTDI.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\Efabless\caravel_board\hardware\caravel_pcb_v3_FTDI\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\Efabless\caravel_board\hardware\caravel_pcb_v4_FTDI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F5F35BB-A34F-427D-AAB8-3F18E5FDBD6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD6D4D97-E662-414F-8063-2A91C3A5D7B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2960" yWindow="2960" windowWidth="19200" windowHeight="11170" xr2:uid="{DBB590BE-7B6D-5543-BF5E-2321E179B520}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{DBB590BE-7B6D-5543-BF5E-2321E179B520}"/>
   </bookViews>
   <sheets>
     <sheet name="BOM" sheetId="3" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="56">
   <si>
     <t>U6</t>
   </si>
@@ -42,9 +42,6 @@
     <t>U1</t>
   </si>
   <si>
-    <t>AZ1117CH-1.8TRG1</t>
-  </si>
-  <si>
     <t>X1</t>
   </si>
   <si>
@@ -81,9 +78,6 @@
     <t>EF</t>
   </si>
   <si>
-    <t>100u</t>
-  </si>
-  <si>
     <t>DK</t>
   </si>
   <si>
@@ -93,24 +87,12 @@
     <t>CC0805KKX5R8BB106</t>
   </si>
   <si>
-    <t>22u</t>
-  </si>
-  <si>
-    <t>1u</t>
-  </si>
-  <si>
-    <t>CC0805MKX5R5BB226</t>
-  </si>
-  <si>
     <t>CC0805KRX7R9BB104</t>
   </si>
   <si>
     <t>0.1u</t>
   </si>
   <si>
-    <t>CC0805KKX7R8BB105</t>
-  </si>
-  <si>
     <t>0.01u</t>
   </si>
   <si>
@@ -162,9 +144,6 @@
     <t>LTST-C230KRKT</t>
   </si>
   <si>
-    <t>GMC31X5R107M6R3NT</t>
-  </si>
-  <si>
     <t>FT232HQ</t>
   </si>
   <si>
@@ -183,33 +162,9 @@
     <t>R3, R4</t>
   </si>
   <si>
-    <t>R1, R5-R10, R12, R13</t>
-  </si>
-  <si>
     <t>C1</t>
   </si>
   <si>
-    <t>C13, C14, C18, C19</t>
-  </si>
-  <si>
-    <t>C16, C17</t>
-  </si>
-  <si>
-    <t>C20, C21</t>
-  </si>
-  <si>
-    <t>C2-C8, C15, C22</t>
-  </si>
-  <si>
-    <t>AZ1117IH-3.3TRG1</t>
-  </si>
-  <si>
-    <t>LDI1117-3.3H</t>
-  </si>
-  <si>
-    <t>C9-C12</t>
-  </si>
-  <si>
     <t>D1, D2, D3, D4</t>
   </si>
   <si>
@@ -220,6 +175,30 @@
   </si>
   <si>
     <t>36-5000-ND</t>
+  </si>
+  <si>
+    <t>MCP1319MT-29LE/OT</t>
+  </si>
+  <si>
+    <t>MIC5350-SGYMT-TR</t>
+  </si>
+  <si>
+    <t>C2-C9, C11, C14, C15</t>
+  </si>
+  <si>
+    <t>2.2u</t>
+  </si>
+  <si>
+    <t>C10</t>
+  </si>
+  <si>
+    <t>C12, C13</t>
+  </si>
+  <si>
+    <t>CC0805KRX5R6BB225</t>
+  </si>
+  <si>
+    <t>R1, R5-R10, R12, R13, R15, R16</t>
   </si>
 </sst>
 </file>
@@ -306,7 +285,7 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -329,9 +308,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyBorder="1"/>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
@@ -650,10 +626,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{718CFFD5-71E2-E44C-BCD6-97EE3DEEFA9F}">
-  <dimension ref="A1:G22"/>
+  <dimension ref="A1:G20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5"/>
@@ -666,19 +642,19 @@
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:7">
@@ -690,66 +666,62 @@
       </c>
       <c r="C2" s="2"/>
       <c r="D2" s="3" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
     </row>
     <row r="3" spans="1:7">
       <c r="A3" s="2" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="B3" s="6">
         <v>2</v>
       </c>
       <c r="C3" s="2"/>
       <c r="D3" s="10" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
     </row>
     <row r="4" spans="1:7">
       <c r="A4" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B4" s="6">
         <v>1</v>
       </c>
       <c r="C4" s="2"/>
       <c r="D4" s="10" t="s">
-        <v>3</v>
+        <v>49</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="F4" s="2"/>
     </row>
     <row r="5" spans="1:7">
       <c r="A5" s="2" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="B5" s="6">
         <v>1</v>
       </c>
       <c r="C5" s="2"/>
       <c r="D5" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="E5" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="G5" s="8" t="s">
-        <v>57</v>
-      </c>
+        <v>48</v>
+      </c>
+      <c r="E5" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="F5" s="2"/>
+      <c r="G5" s="8"/>
     </row>
     <row r="6" spans="1:7">
       <c r="A6" s="2" t="s">
@@ -763,105 +735,104 @@
         <v>1</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="7" spans="1:7">
       <c r="A7" s="2" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="B7" s="6">
         <v>1</v>
       </c>
       <c r="C7" s="2"/>
       <c r="D7" s="8" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" t="s">
-        <v>59</v>
+        <v>44</v>
       </c>
       <c r="B8" s="7">
         <v>4</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="E8" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="9" spans="1:7">
       <c r="A9" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="B9" s="7">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C9" t="s">
         <v>16</v>
       </c>
-      <c r="D9" s="9" t="s">
-        <v>43</v>
+      <c r="D9" s="8" t="s">
+        <v>17</v>
       </c>
       <c r="E9" t="s">
-        <v>17</v>
-      </c>
-      <c r="F9" s="8"/>
+        <v>15</v>
+      </c>
     </row>
     <row r="10" spans="1:7">
       <c r="A10" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B10" s="7">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C10" t="s">
-        <v>18</v>
-      </c>
-      <c r="D10" s="8" t="s">
-        <v>19</v>
+        <v>51</v>
+      </c>
+      <c r="D10" s="10" t="s">
+        <v>54</v>
       </c>
       <c r="E10" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="11" spans="1:7">
       <c r="A11" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="B11" s="7">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="C11" t="s">
-        <v>20</v>
-      </c>
-      <c r="D11" s="10" t="s">
-        <v>22</v>
+        <v>19</v>
+      </c>
+      <c r="D11" s="9" t="s">
+        <v>18</v>
       </c>
       <c r="E11" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="12" spans="1:7">
       <c r="A12" t="s">
-        <v>54</v>
+        <v>43</v>
       </c>
       <c r="B12" s="7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C12" t="s">
+        <v>20</v>
+      </c>
+      <c r="D12" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="D12" s="11" t="s">
-        <v>25</v>
-      </c>
       <c r="E12" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="13" spans="1:7">
@@ -869,189 +840,152 @@
         <v>55</v>
       </c>
       <c r="B13" s="7">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C13" t="s">
-        <v>24</v>
-      </c>
-      <c r="D13" s="9" t="s">
         <v>23</v>
       </c>
+      <c r="D13" s="8" t="s">
+        <v>22</v>
+      </c>
       <c r="E13" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="14" spans="1:7">
       <c r="A14" t="s">
-        <v>51</v>
+        <v>41</v>
       </c>
       <c r="B14" s="7">
         <v>1</v>
       </c>
       <c r="C14" t="s">
-        <v>26</v>
-      </c>
-      <c r="D14" s="10" t="s">
-        <v>27</v>
+        <v>24</v>
+      </c>
+      <c r="D14" s="9" t="s">
+        <v>35</v>
       </c>
       <c r="E14" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="15" spans="1:7">
       <c r="A15" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="B15" s="7">
-        <v>9</v>
-      </c>
-      <c r="C15" t="s">
-        <v>29</v>
+        <v>2</v>
+      </c>
+      <c r="C15" s="4">
+        <v>150</v>
       </c>
       <c r="D15" s="8" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="E15" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="16" spans="1:7">
       <c r="A16" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B16" s="7">
-        <v>1</v>
-      </c>
-      <c r="C16" t="s">
-        <v>30</v>
+        <v>2</v>
+      </c>
+      <c r="C16" s="4">
+        <v>82</v>
       </c>
       <c r="D16" s="9" t="s">
-        <v>41</v>
+        <v>26</v>
       </c>
       <c r="E16" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="17" spans="1:5">
       <c r="A17" t="s">
-        <v>49</v>
+        <v>6</v>
       </c>
       <c r="B17" s="7">
-        <v>2</v>
-      </c>
-      <c r="C17" s="4">
-        <v>150</v>
+        <v>1</v>
       </c>
       <c r="D17" s="8" t="s">
         <v>31</v>
       </c>
       <c r="E17" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="18" spans="1:5">
       <c r="A18" t="s">
-        <v>60</v>
+        <v>3</v>
       </c>
       <c r="B18" s="7">
-        <v>2</v>
-      </c>
-      <c r="C18" s="4">
-        <v>82</v>
-      </c>
-      <c r="D18" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="C18" t="s">
+        <v>34</v>
+      </c>
+      <c r="D18" s="10" t="s">
         <v>32</v>
       </c>
       <c r="E18" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="19" spans="1:5">
       <c r="A19" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B19" s="7">
         <v>1</v>
       </c>
-      <c r="D19" s="8" t="s">
-        <v>37</v>
+      <c r="C19" t="s">
+        <v>33</v>
+      </c>
+      <c r="D19" s="10" t="s">
+        <v>5</v>
       </c>
       <c r="E19" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="20" spans="1:5">
       <c r="A20" t="s">
-        <v>4</v>
+        <v>46</v>
       </c>
       <c r="B20" s="7">
-        <v>1</v>
-      </c>
-      <c r="C20" t="s">
-        <v>40</v>
+        <v>2</v>
       </c>
       <c r="D20" s="10" t="s">
-        <v>38</v>
+        <v>47</v>
       </c>
       <c r="E20" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5">
-      <c r="A21" t="s">
-        <v>5</v>
-      </c>
-      <c r="B21" s="7">
-        <v>1</v>
-      </c>
-      <c r="C21" t="s">
-        <v>39</v>
-      </c>
-      <c r="D21" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="E21" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5">
-      <c r="A22" t="s">
-        <v>61</v>
-      </c>
-      <c r="B22" s="7">
-        <v>2</v>
-      </c>
-      <c r="D22" s="10" t="s">
-        <v>62</v>
-      </c>
-      <c r="E22" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D9" r:id="rId1" display="https://www.digikey.com/en/products/detail/cal-chip-electronics-inc/GMC31X5R107M6R3NT/12140450" xr:uid="{59A69107-AC02-324B-BC04-998787DA3D4E}"/>
-    <hyperlink ref="D3" r:id="rId2" xr:uid="{15EAEAB6-A0CB-4ACF-8CD3-161025C29E44}"/>
-    <hyperlink ref="D4" r:id="rId3" xr:uid="{747FE5E0-2A4E-4068-AB0D-CAC39D5826C7}"/>
-    <hyperlink ref="D7" r:id="rId4" xr:uid="{4D5C5894-AC8C-4FCC-B89B-BB8697C65FB3}"/>
-    <hyperlink ref="D8" r:id="rId5" xr:uid="{FBD05251-0C7B-4F92-89D7-CB9A16D0196A}"/>
-    <hyperlink ref="D10" r:id="rId6" xr:uid="{E464CA61-42F7-44EB-BF01-8B800CA45EF3}"/>
-    <hyperlink ref="D11" r:id="rId7" xr:uid="{88880D05-CE4C-4553-B5B7-2F3974B403A0}"/>
-    <hyperlink ref="D12" r:id="rId8" xr:uid="{A166FDAB-845F-414C-A5AF-38BED4FEA5F6}"/>
-    <hyperlink ref="D13" r:id="rId9" xr:uid="{C58D724D-09D3-4878-B2B2-C057FE7EBF98}"/>
-    <hyperlink ref="D14" r:id="rId10" xr:uid="{F6494E5B-794F-443D-8BCB-774F2B018876}"/>
-    <hyperlink ref="D15" r:id="rId11" xr:uid="{ABAA75D8-8BBB-487E-B8B1-3C0AF7EB0A3B}"/>
-    <hyperlink ref="D16" r:id="rId12" xr:uid="{32B4110F-CB40-49D0-B0EC-DF2656A41CB0}"/>
-    <hyperlink ref="D17" r:id="rId13" xr:uid="{45E79B76-DA2E-4118-8AFE-B36E33A83B39}"/>
-    <hyperlink ref="D18" r:id="rId14" xr:uid="{CC7D2AB0-FD93-4356-BB92-AC66D6DD8CB8}"/>
-    <hyperlink ref="D19" r:id="rId15" xr:uid="{ECA5F3D5-98AA-46FB-B542-A4223E5D1F67}"/>
-    <hyperlink ref="D20" r:id="rId16" xr:uid="{D0C57109-E46E-4775-A78E-2E4F393E4DB0}"/>
-    <hyperlink ref="D21" r:id="rId17" xr:uid="{1F484673-4C77-4CD6-8F13-F5756E1F14E9}"/>
-    <hyperlink ref="D5" r:id="rId18" xr:uid="{AC4A8384-9698-417E-B845-F4D6E4DAD7D2}"/>
-    <hyperlink ref="G5" r:id="rId19" xr:uid="{D63976FF-547D-46FE-8D03-6E293B2A60F9}"/>
-    <hyperlink ref="D22" r:id="rId20" xr:uid="{77AF3B6F-44B4-4877-A203-88B8BD419D7C}"/>
+    <hyperlink ref="D3" r:id="rId1" xr:uid="{15EAEAB6-A0CB-4ACF-8CD3-161025C29E44}"/>
+    <hyperlink ref="D7" r:id="rId2" xr:uid="{4D5C5894-AC8C-4FCC-B89B-BB8697C65FB3}"/>
+    <hyperlink ref="D8" r:id="rId3" xr:uid="{FBD05251-0C7B-4F92-89D7-CB9A16D0196A}"/>
+    <hyperlink ref="D9" r:id="rId4" xr:uid="{E464CA61-42F7-44EB-BF01-8B800CA45EF3}"/>
+    <hyperlink ref="D11" r:id="rId5" xr:uid="{C58D724D-09D3-4878-B2B2-C057FE7EBF98}"/>
+    <hyperlink ref="D12" r:id="rId6" xr:uid="{F6494E5B-794F-443D-8BCB-774F2B018876}"/>
+    <hyperlink ref="D13" r:id="rId7" xr:uid="{ABAA75D8-8BBB-487E-B8B1-3C0AF7EB0A3B}"/>
+    <hyperlink ref="D14" r:id="rId8" xr:uid="{32B4110F-CB40-49D0-B0EC-DF2656A41CB0}"/>
+    <hyperlink ref="D15" r:id="rId9" xr:uid="{45E79B76-DA2E-4118-8AFE-B36E33A83B39}"/>
+    <hyperlink ref="D16" r:id="rId10" xr:uid="{CC7D2AB0-FD93-4356-BB92-AC66D6DD8CB8}"/>
+    <hyperlink ref="D17" r:id="rId11" xr:uid="{ECA5F3D5-98AA-46FB-B542-A4223E5D1F67}"/>
+    <hyperlink ref="D18" r:id="rId12" xr:uid="{D0C57109-E46E-4775-A78E-2E4F393E4DB0}"/>
+    <hyperlink ref="D19" r:id="rId13" xr:uid="{1F484673-4C77-4CD6-8F13-F5756E1F14E9}"/>
+    <hyperlink ref="D20" r:id="rId14" xr:uid="{77AF3B6F-44B4-4877-A203-88B8BD419D7C}"/>
+    <hyperlink ref="D5" r:id="rId15" xr:uid="{65576AB4-FE37-4502-A8BE-265FF7E9ABF9}"/>
+    <hyperlink ref="D4" r:id="rId16" xr:uid="{B6DDCD80-0F01-49EF-A92E-806CE584A9CD}"/>
+    <hyperlink ref="D10" r:id="rId17" xr:uid="{CD641C67-9878-4576-8449-0A3B0EB06D7C}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId21"/>
+  <pageSetup orientation="portrait" r:id="rId18"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
update caravel FTDI mainboard V4 (Rev 4B) to support different LDO devices with the same footprint
</commit_message>
<xml_diff>
--- a/hardware/caravel_pcb_v4_FTDI/caravel_pcb_v4_FTDI.xlsx
+++ b/hardware/caravel_pcb_v4_FTDI/caravel_pcb_v4_FTDI.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\Efabless\caravel_board\hardware\caravel_pcb_v4_FTDI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD6D4D97-E662-414F-8063-2A91C3A5D7B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2CD696B-2903-432E-AAF9-DC34E1621F15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{DBB590BE-7B6D-5543-BF5E-2321E179B520}"/>
+    <workbookView xWindow="2960" yWindow="2960" windowWidth="19200" windowHeight="11170" xr2:uid="{DBB590BE-7B6D-5543-BF5E-2321E179B520}"/>
   </bookViews>
   <sheets>
     <sheet name="BOM" sheetId="3" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="58">
   <si>
     <t>U6</t>
   </si>
@@ -153,18 +153,12 @@
     <t>U7</t>
   </si>
   <si>
-    <t xml:space="preserve">U5 </t>
-  </si>
-  <si>
     <t>R2</t>
   </si>
   <si>
     <t>R3, R4</t>
   </si>
   <si>
-    <t>C1</t>
-  </si>
-  <si>
     <t>D1, D2, D3, D4</t>
   </si>
   <si>
@@ -180,25 +174,37 @@
     <t>MCP1319MT-29LE/OT</t>
   </si>
   <si>
-    <t>MIC5350-SGYMT-TR</t>
-  </si>
-  <si>
-    <t>C2-C9, C11, C14, C15</t>
-  </si>
-  <si>
-    <t>2.2u</t>
-  </si>
-  <si>
-    <t>C10</t>
-  </si>
-  <si>
-    <t>C12, C13</t>
-  </si>
-  <si>
-    <t>CC0805KRX5R6BB225</t>
-  </si>
-  <si>
     <t>R1, R5-R10, R12, R13, R15, R16</t>
+  </si>
+  <si>
+    <t>U5</t>
+  </si>
+  <si>
+    <t>TAR5S33UTE85LF</t>
+  </si>
+  <si>
+    <t>U8</t>
+  </si>
+  <si>
+    <t>TAR5S18UTE85LF or TAR5S16UTE85L</t>
+  </si>
+  <si>
+    <t>1u</t>
+  </si>
+  <si>
+    <t>C1, C11, C14</t>
+  </si>
+  <si>
+    <t>C12, C15</t>
+  </si>
+  <si>
+    <t>C10, C13</t>
+  </si>
+  <si>
+    <t>C2-C9, C16, C17</t>
+  </si>
+  <si>
+    <t>CC0805KKX7R7BB105</t>
   </si>
 </sst>
 </file>
@@ -626,10 +632,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{718CFFD5-71E2-E44C-BCD6-97EE3DEEFA9F}">
-  <dimension ref="A1:G20"/>
+  <dimension ref="A1:G21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="A9" sqref="A9:XFD9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5"/>
@@ -698,45 +704,45 @@
         <v>1</v>
       </c>
       <c r="C4" s="2"/>
-      <c r="D4" s="10" t="s">
-        <v>49</v>
-      </c>
-      <c r="E4" s="2" t="s">
+      <c r="D4" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="E4" s="11" t="s">
         <v>15</v>
       </c>
       <c r="F4" s="2"/>
     </row>
     <row r="5" spans="1:7">
       <c r="A5" s="2" t="s">
-        <v>40</v>
+        <v>48</v>
       </c>
       <c r="B5" s="6">
         <v>1</v>
       </c>
       <c r="C5" s="2"/>
       <c r="D5" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="E5" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="E5" s="2" t="s">
         <v>15</v>
       </c>
       <c r="F5" s="2"/>
-      <c r="G5" s="8"/>
     </row>
     <row r="6" spans="1:7">
       <c r="A6" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="6">
+      <c r="B6" s="7">
         <v>1</v>
       </c>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2" t="s">
-        <v>1</v>
+      <c r="D6" s="8" t="s">
+        <v>51</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>14</v>
-      </c>
+        <v>15</v>
+      </c>
+      <c r="F6" s="2"/>
+      <c r="G6" s="8"/>
     </row>
     <row r="7" spans="1:7">
       <c r="A7" s="2" t="s">
@@ -754,31 +760,29 @@
       </c>
     </row>
     <row r="8" spans="1:7">
-      <c r="A8" t="s">
-        <v>44</v>
-      </c>
-      <c r="B8" s="7">
-        <v>4</v>
-      </c>
-      <c r="D8" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="E8" t="s">
-        <v>15</v>
+      <c r="A8" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B8" s="6">
+        <v>1</v>
+      </c>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="9" spans="1:7">
       <c r="A9" t="s">
-        <v>52</v>
+        <v>42</v>
       </c>
       <c r="B9" s="7">
-        <v>1</v>
-      </c>
-      <c r="C9" t="s">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="D9" s="8" t="s">
-        <v>17</v>
+        <v>36</v>
       </c>
       <c r="E9" t="s">
         <v>15</v>
@@ -786,16 +790,16 @@
     </row>
     <row r="10" spans="1:7">
       <c r="A10" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B10" s="7">
         <v>2</v>
       </c>
       <c r="C10" t="s">
-        <v>51</v>
-      </c>
-      <c r="D10" s="10" t="s">
-        <v>54</v>
+        <v>16</v>
+      </c>
+      <c r="D10" s="8" t="s">
+        <v>17</v>
       </c>
       <c r="E10" t="s">
         <v>15</v>
@@ -803,16 +807,16 @@
     </row>
     <row r="11" spans="1:7">
       <c r="A11" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="B11" s="7">
-        <v>11</v>
+        <v>2</v>
       </c>
       <c r="C11" t="s">
-        <v>19</v>
-      </c>
-      <c r="D11" s="9" t="s">
-        <v>18</v>
+        <v>52</v>
+      </c>
+      <c r="D11" s="8" t="s">
+        <v>57</v>
       </c>
       <c r="E11" t="s">
         <v>15</v>
@@ -820,16 +824,16 @@
     </row>
     <row r="12" spans="1:7">
       <c r="A12" t="s">
-        <v>43</v>
+        <v>56</v>
       </c>
       <c r="B12" s="7">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="C12" t="s">
-        <v>20</v>
-      </c>
-      <c r="D12" s="10" t="s">
-        <v>21</v>
+        <v>19</v>
+      </c>
+      <c r="D12" s="9" t="s">
+        <v>18</v>
       </c>
       <c r="E12" t="s">
         <v>15</v>
@@ -837,16 +841,16 @@
     </row>
     <row r="13" spans="1:7">
       <c r="A13" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B13" s="7">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="C13" t="s">
-        <v>23</v>
-      </c>
-      <c r="D13" s="8" t="s">
-        <v>22</v>
+        <v>20</v>
+      </c>
+      <c r="D13" s="10" t="s">
+        <v>21</v>
       </c>
       <c r="E13" t="s">
         <v>15</v>
@@ -854,16 +858,16 @@
     </row>
     <row r="14" spans="1:7">
       <c r="A14" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="B14" s="7">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="C14" t="s">
-        <v>24</v>
-      </c>
-      <c r="D14" s="9" t="s">
-        <v>35</v>
+        <v>23</v>
+      </c>
+      <c r="D14" s="8" t="s">
+        <v>22</v>
       </c>
       <c r="E14" t="s">
         <v>15</v>
@@ -871,16 +875,16 @@
     </row>
     <row r="15" spans="1:7">
       <c r="A15" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B15" s="7">
-        <v>2</v>
-      </c>
-      <c r="C15" s="4">
-        <v>150</v>
-      </c>
-      <c r="D15" s="8" t="s">
-        <v>25</v>
+        <v>1</v>
+      </c>
+      <c r="C15" t="s">
+        <v>24</v>
+      </c>
+      <c r="D15" s="9" t="s">
+        <v>35</v>
       </c>
       <c r="E15" t="s">
         <v>15</v>
@@ -888,16 +892,16 @@
     </row>
     <row r="16" spans="1:7">
       <c r="A16" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="B16" s="7">
         <v>2</v>
       </c>
       <c r="C16" s="4">
-        <v>82</v>
-      </c>
-      <c r="D16" s="9" t="s">
-        <v>26</v>
+        <v>150</v>
+      </c>
+      <c r="D16" s="8" t="s">
+        <v>25</v>
       </c>
       <c r="E16" t="s">
         <v>15</v>
@@ -905,13 +909,16 @@
     </row>
     <row r="17" spans="1:5">
       <c r="A17" t="s">
-        <v>6</v>
+        <v>43</v>
       </c>
       <c r="B17" s="7">
-        <v>1</v>
-      </c>
-      <c r="D17" s="8" t="s">
-        <v>31</v>
+        <v>2</v>
+      </c>
+      <c r="C17" s="4">
+        <v>82</v>
+      </c>
+      <c r="D17" s="9" t="s">
+        <v>26</v>
       </c>
       <c r="E17" t="s">
         <v>15</v>
@@ -919,16 +926,13 @@
     </row>
     <row r="18" spans="1:5">
       <c r="A18" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="B18" s="7">
         <v>1</v>
       </c>
-      <c r="C18" t="s">
-        <v>34</v>
-      </c>
-      <c r="D18" s="10" t="s">
-        <v>32</v>
+      <c r="D18" s="8" t="s">
+        <v>31</v>
       </c>
       <c r="E18" t="s">
         <v>15</v>
@@ -936,16 +940,16 @@
     </row>
     <row r="19" spans="1:5">
       <c r="A19" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B19" s="7">
         <v>1</v>
       </c>
       <c r="C19" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D19" s="10" t="s">
-        <v>5</v>
+        <v>32</v>
       </c>
       <c r="E19" t="s">
         <v>15</v>
@@ -953,15 +957,32 @@
     </row>
     <row r="20" spans="1:5">
       <c r="A20" t="s">
-        <v>46</v>
+        <v>4</v>
       </c>
       <c r="B20" s="7">
+        <v>1</v>
+      </c>
+      <c r="C20" t="s">
+        <v>33</v>
+      </c>
+      <c r="D20" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="E20" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5">
+      <c r="A21" t="s">
+        <v>44</v>
+      </c>
+      <c r="B21" s="7">
         <v>2</v>
       </c>
-      <c r="D20" s="10" t="s">
-        <v>47</v>
-      </c>
-      <c r="E20" t="s">
+      <c r="D21" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="E21" t="s">
         <v>15</v>
       </c>
     </row>
@@ -969,23 +990,24 @@
   <hyperlinks>
     <hyperlink ref="D3" r:id="rId1" xr:uid="{15EAEAB6-A0CB-4ACF-8CD3-161025C29E44}"/>
     <hyperlink ref="D7" r:id="rId2" xr:uid="{4D5C5894-AC8C-4FCC-B89B-BB8697C65FB3}"/>
-    <hyperlink ref="D8" r:id="rId3" xr:uid="{FBD05251-0C7B-4F92-89D7-CB9A16D0196A}"/>
-    <hyperlink ref="D9" r:id="rId4" xr:uid="{E464CA61-42F7-44EB-BF01-8B800CA45EF3}"/>
-    <hyperlink ref="D11" r:id="rId5" xr:uid="{C58D724D-09D3-4878-B2B2-C057FE7EBF98}"/>
-    <hyperlink ref="D12" r:id="rId6" xr:uid="{F6494E5B-794F-443D-8BCB-774F2B018876}"/>
-    <hyperlink ref="D13" r:id="rId7" xr:uid="{ABAA75D8-8BBB-487E-B8B1-3C0AF7EB0A3B}"/>
-    <hyperlink ref="D14" r:id="rId8" xr:uid="{32B4110F-CB40-49D0-B0EC-DF2656A41CB0}"/>
-    <hyperlink ref="D15" r:id="rId9" xr:uid="{45E79B76-DA2E-4118-8AFE-B36E33A83B39}"/>
-    <hyperlink ref="D16" r:id="rId10" xr:uid="{CC7D2AB0-FD93-4356-BB92-AC66D6DD8CB8}"/>
-    <hyperlink ref="D17" r:id="rId11" xr:uid="{ECA5F3D5-98AA-46FB-B542-A4223E5D1F67}"/>
-    <hyperlink ref="D18" r:id="rId12" xr:uid="{D0C57109-E46E-4775-A78E-2E4F393E4DB0}"/>
-    <hyperlink ref="D19" r:id="rId13" xr:uid="{1F484673-4C77-4CD6-8F13-F5756E1F14E9}"/>
-    <hyperlink ref="D20" r:id="rId14" xr:uid="{77AF3B6F-44B4-4877-A203-88B8BD419D7C}"/>
-    <hyperlink ref="D5" r:id="rId15" xr:uid="{65576AB4-FE37-4502-A8BE-265FF7E9ABF9}"/>
-    <hyperlink ref="D4" r:id="rId16" xr:uid="{B6DDCD80-0F01-49EF-A92E-806CE584A9CD}"/>
-    <hyperlink ref="D10" r:id="rId17" xr:uid="{CD641C67-9878-4576-8449-0A3B0EB06D7C}"/>
+    <hyperlink ref="D9" r:id="rId3" xr:uid="{FBD05251-0C7B-4F92-89D7-CB9A16D0196A}"/>
+    <hyperlink ref="D12" r:id="rId4" xr:uid="{C58D724D-09D3-4878-B2B2-C057FE7EBF98}"/>
+    <hyperlink ref="D13" r:id="rId5" xr:uid="{F6494E5B-794F-443D-8BCB-774F2B018876}"/>
+    <hyperlink ref="D14" r:id="rId6" xr:uid="{ABAA75D8-8BBB-487E-B8B1-3C0AF7EB0A3B}"/>
+    <hyperlink ref="D15" r:id="rId7" xr:uid="{32B4110F-CB40-49D0-B0EC-DF2656A41CB0}"/>
+    <hyperlink ref="D16" r:id="rId8" xr:uid="{45E79B76-DA2E-4118-8AFE-B36E33A83B39}"/>
+    <hyperlink ref="D17" r:id="rId9" xr:uid="{CC7D2AB0-FD93-4356-BB92-AC66D6DD8CB8}"/>
+    <hyperlink ref="D18" r:id="rId10" xr:uid="{ECA5F3D5-98AA-46FB-B542-A4223E5D1F67}"/>
+    <hyperlink ref="D19" r:id="rId11" xr:uid="{D0C57109-E46E-4775-A78E-2E4F393E4DB0}"/>
+    <hyperlink ref="D20" r:id="rId12" xr:uid="{1F484673-4C77-4CD6-8F13-F5756E1F14E9}"/>
+    <hyperlink ref="D21" r:id="rId13" xr:uid="{77AF3B6F-44B4-4877-A203-88B8BD419D7C}"/>
+    <hyperlink ref="D4" r:id="rId14" xr:uid="{65576AB4-FE37-4502-A8BE-265FF7E9ABF9}"/>
+    <hyperlink ref="D6" r:id="rId15" xr:uid="{2127627C-7017-42FB-8DA8-E679BFB4E758}"/>
+    <hyperlink ref="D5" r:id="rId16" xr:uid="{4A73DBD0-B5FB-4EA1-A7E5-13DF03ABC85B}"/>
+    <hyperlink ref="D10" r:id="rId17" xr:uid="{E464CA61-42F7-44EB-BF01-8B800CA45EF3}"/>
+    <hyperlink ref="D11" r:id="rId18" xr:uid="{BD6CFC13-E75A-43AB-8083-A44296ED7D4B}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId18"/>
+  <pageSetup orientation="portrait" r:id="rId19"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
update BOM caravel FTDI mainboard V4 (Rev 4B)
</commit_message>
<xml_diff>
--- a/hardware/caravel_pcb_v4_FTDI/caravel_pcb_v4_FTDI.xlsx
+++ b/hardware/caravel_pcb_v4_FTDI/caravel_pcb_v4_FTDI.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\Efabless\caravel_board\hardware\caravel_pcb_v4_FTDI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2CD696B-2903-432E-AAF9-DC34E1621F15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41750F50-E64B-42E4-AE33-63720122C312}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2960" yWindow="2960" windowWidth="19200" windowHeight="11170" xr2:uid="{DBB590BE-7B6D-5543-BF5E-2321E179B520}"/>
   </bookViews>
@@ -186,9 +186,6 @@
     <t>U8</t>
   </si>
   <si>
-    <t>TAR5S18UTE85LF or TAR5S16UTE85L</t>
-  </si>
-  <si>
     <t>1u</t>
   </si>
   <si>
@@ -205,6 +202,9 @@
   </si>
   <si>
     <t>CC0805KKX7R7BB105</t>
+  </si>
+  <si>
+    <t>TAR5S16UTE85LF</t>
   </si>
 </sst>
 </file>
@@ -635,7 +635,7 @@
   <dimension ref="A1:G21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9:XFD9"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5"/>
@@ -736,7 +736,7 @@
         <v>1</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>51</v>
+        <v>57</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>15</v>
@@ -790,7 +790,7 @@
     </row>
     <row r="10" spans="1:7">
       <c r="A10" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B10" s="7">
         <v>2</v>
@@ -807,16 +807,16 @@
     </row>
     <row r="11" spans="1:7">
       <c r="A11" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B11" s="7">
         <v>2</v>
       </c>
       <c r="C11" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D11" s="8" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E11" t="s">
         <v>15</v>
@@ -824,7 +824,7 @@
     </row>
     <row r="12" spans="1:7">
       <c r="A12" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B12" s="7">
         <v>10</v>
@@ -841,7 +841,7 @@
     </row>
     <row r="13" spans="1:7">
       <c r="A13" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B13" s="7">
         <v>3</v>
@@ -1002,7 +1002,7 @@
     <hyperlink ref="D20" r:id="rId12" xr:uid="{1F484673-4C77-4CD6-8F13-F5756E1F14E9}"/>
     <hyperlink ref="D21" r:id="rId13" xr:uid="{77AF3B6F-44B4-4877-A203-88B8BD419D7C}"/>
     <hyperlink ref="D4" r:id="rId14" xr:uid="{65576AB4-FE37-4502-A8BE-265FF7E9ABF9}"/>
-    <hyperlink ref="D6" r:id="rId15" xr:uid="{2127627C-7017-42FB-8DA8-E679BFB4E758}"/>
+    <hyperlink ref="D6" r:id="rId15" display="TAR5S16UTE85L" xr:uid="{2127627C-7017-42FB-8DA8-E679BFB4E758}"/>
     <hyperlink ref="D5" r:id="rId16" xr:uid="{4A73DBD0-B5FB-4EA1-A7E5-13DF03ABC85B}"/>
     <hyperlink ref="D10" r:id="rId17" xr:uid="{E464CA61-42F7-44EB-BF01-8B800CA45EF3}"/>
     <hyperlink ref="D11" r:id="rId18" xr:uid="{BD6CFC13-E75A-43AB-8083-A44296ED7D4B}"/>

</xml_diff>